<commit_message>
create_user_test test case and data added
</commit_message>
<xml_diff>
--- a/TestData/Users.xlsx
+++ b/TestData/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\Downloads\PetStoreTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183FE0AD-BDF7-4FCC-B6D9-B62734513521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60653E0A-5982-4F5B-9CAA-F645EE66614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
   <si>
     <t>action</t>
   </si>
@@ -58,13 +58,274 @@
   </si>
   <si>
     <t>create_user_test</t>
+  </si>
+  <si>
+    <t>abcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcdabcd</t>
+  </si>
+  <si>
+    <t>tquirke0</t>
+  </si>
+  <si>
+    <t>Thom</t>
+  </si>
+  <si>
+    <t>Quirke</t>
+  </si>
+  <si>
+    <t>tquirke0@si.edu</t>
+  </si>
+  <si>
+    <t>bR0"ZkydOOA$</t>
+  </si>
+  <si>
+    <t>259-873-7141</t>
+  </si>
+  <si>
+    <t>Purcell</t>
+  </si>
+  <si>
+    <t>Harcombe</t>
+  </si>
+  <si>
+    <t>pharcombe1@cmu.edu</t>
+  </si>
+  <si>
+    <t>vS8}&amp;&amp;6?|</t>
+  </si>
+  <si>
+    <t>893-763-3832</t>
+  </si>
+  <si>
+    <t>Rosenthaler</t>
+  </si>
+  <si>
+    <t>grosenthaler2@kickstarter.com</t>
+  </si>
+  <si>
+    <t>dF7.q|toR</t>
+  </si>
+  <si>
+    <t>423-874-5599</t>
+  </si>
+  <si>
+    <t>Dian</t>
+  </si>
+  <si>
+    <t>dbunkle3@amazon.de</t>
+  </si>
+  <si>
+    <t>fY4_sXZx=Y%0</t>
+  </si>
+  <si>
+    <t>115-641-4814</t>
+  </si>
+  <si>
+    <t>Marabel</t>
+  </si>
+  <si>
+    <t>Brixey</t>
+  </si>
+  <si>
+    <t>tG6+Xynk7@K,J$'</t>
+  </si>
+  <si>
+    <t>519-444-7692</t>
+  </si>
+  <si>
+    <t>Jewel</t>
+  </si>
+  <si>
+    <t>Rosenbloom</t>
+  </si>
+  <si>
+    <t>jrosenbloom5@booking.com</t>
+  </si>
+  <si>
+    <t>928-410-9006</t>
+  </si>
+  <si>
+    <t>Katti</t>
+  </si>
+  <si>
+    <t>Bearham</t>
+  </si>
+  <si>
+    <t>kbearham6@chicagotribune.com</t>
+  </si>
+  <si>
+    <t>mF6"IZ(yxk</t>
+  </si>
+  <si>
+    <t>grosenthaler2</t>
+  </si>
+  <si>
+    <t>dbunkle3</t>
+  </si>
+  <si>
+    <t>mbrixey4</t>
+  </si>
+  <si>
+    <t>jrosenbloom5</t>
+  </si>
+  <si>
+    <t>kbearham6</t>
+  </si>
+  <si>
+    <t>%^&amp;%^&amp;%^&amp;</t>
+  </si>
+  <si>
+    <t>gsture7</t>
+  </si>
+  <si>
+    <t>Galvin</t>
+  </si>
+  <si>
+    <t>Sture</t>
+  </si>
+  <si>
+    <t>gsture7@alexa.com</t>
+  </si>
+  <si>
+    <t>uB5=QdTt.2zyG}CZ</t>
+  </si>
+  <si>
+    <t>712-347-5792</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>clehuquet8</t>
+  </si>
+  <si>
+    <t>Caria</t>
+  </si>
+  <si>
+    <t>Le Huquet</t>
+  </si>
+  <si>
+    <t>clehuquet8@nytimes.com</t>
+  </si>
+  <si>
+    <t>tL0"KbJHj8&lt;OU'0</t>
+  </si>
+  <si>
+    <t>213-890-7899</t>
+  </si>
+  <si>
+    <t>Jenna</t>
+  </si>
+  <si>
+    <t>McAnellye</t>
+  </si>
+  <si>
+    <t>jmcanellye9@npr.org</t>
+  </si>
+  <si>
+    <t>pO8_\lZf+)</t>
+  </si>
+  <si>
+    <t>554-381-9620</t>
+  </si>
+  <si>
+    <t>pelfleeta</t>
+  </si>
+  <si>
+    <t>Elfleet</t>
+  </si>
+  <si>
+    <t>pelfleeta@marriott.com</t>
+  </si>
+  <si>
+    <t>rP2}&gt;\(8/o</t>
+  </si>
+  <si>
+    <t>518-845-6484</t>
+  </si>
+  <si>
+    <t>kbulstrodeb</t>
+  </si>
+  <si>
+    <t>Kalli</t>
+  </si>
+  <si>
+    <t>kbulstrodeb@microsoft.com</t>
+  </si>
+  <si>
+    <t>cF6*4bdTA</t>
+  </si>
+  <si>
+    <t>315-881-9458</t>
+  </si>
+  <si>
+    <t>pburstowc</t>
+  </si>
+  <si>
+    <t>Priscella</t>
+  </si>
+  <si>
+    <t>Burstow</t>
+  </si>
+  <si>
+    <t>hN2#6U%uS</t>
+  </si>
+  <si>
+    <t>198-417-1859</t>
+  </si>
+  <si>
+    <t>dlorenzod</t>
+  </si>
+  <si>
+    <t>Danyette</t>
+  </si>
+  <si>
+    <t>Lorenzo</t>
+  </si>
+  <si>
+    <t>dlorenzod@unc.edu</t>
+  </si>
+  <si>
+    <t>124-614-6384</t>
+  </si>
+  <si>
+    <t>jtaskere</t>
+  </si>
+  <si>
+    <t>Jermain</t>
+  </si>
+  <si>
+    <t>Tasker</t>
+  </si>
+  <si>
+    <t>jtaskere@sphinn.com</t>
+  </si>
+  <si>
+    <t>qF4!hk1XTC</t>
+  </si>
+  <si>
+    <t>kgreerf</t>
+  </si>
+  <si>
+    <t>Karalee</t>
+  </si>
+  <si>
+    <t>Greer</t>
+  </si>
+  <si>
+    <t>kgreerf@simplemachines.org</t>
+  </si>
+  <si>
+    <t>iE8\VQ/G</t>
+  </si>
+  <si>
+    <t>958-919-2877</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,30 +334,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FFA9B7C6"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF72737A"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,17 +366,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,88 +658,629 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
         <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="1">
+        <v>6</v>
+      </c>
+      <c r="J9" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="1">
+        <v>7</v>
+      </c>
+      <c r="J10" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="1">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="1">
+        <v>9</v>
+      </c>
+      <c r="J12" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="1">
+        <v>10</v>
+      </c>
+      <c r="J13" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="1">
+        <v>11</v>
+      </c>
+      <c r="J14" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="1">
+        <v>12</v>
+      </c>
+      <c r="J15" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="1">
+        <v>13</v>
+      </c>
+      <c r="J16" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="1">
+        <v>14</v>
+      </c>
+      <c r="J17" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" s="1">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
case and data added
</commit_message>
<xml_diff>
--- a/TestData/Users.xlsx
+++ b/TestData/Users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\Downloads\PetStoreTesting\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60653E0A-5982-4F5B-9CAA-F645EE66614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F18A897-44AC-43A4-B6E7-14437D551DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="114">
   <si>
     <t>action</t>
   </si>
@@ -319,13 +319,61 @@
   </si>
   <si>
     <t>958-919-2877</t>
+  </si>
+  <si>
+    <t>user_login_test</t>
+  </si>
+  <si>
+    <t>ddanahar0</t>
+  </si>
+  <si>
+    <t>aE1*a\WxvWl</t>
+  </si>
+  <si>
+    <t>etucknott1</t>
+  </si>
+  <si>
+    <t>dZ3}AkrHcfH</t>
+  </si>
+  <si>
+    <t>rlevermore2</t>
+  </si>
+  <si>
+    <t>bL5%&lt;kdf/oTbpS&amp;b</t>
+  </si>
+  <si>
+    <t>nnowakowska3</t>
+  </si>
+  <si>
+    <t>eQ7&amp;66}t{</t>
+  </si>
+  <si>
+    <t>hcraggs4</t>
+  </si>
+  <si>
+    <t>nO8"Uq#rPrrBt&gt;</t>
+  </si>
+  <si>
+    <t>get_user_test</t>
+  </si>
+  <si>
+    <t>update_user_test</t>
+  </si>
+  <si>
+    <t>newUsername</t>
+  </si>
+  <si>
+    <t>usernamenotfound</t>
+  </si>
+  <si>
+    <t>delete_user_test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +386,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -363,24 +416,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{0DF44849-E55F-4296-971B-4DA01E082C51}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -658,632 +722,1526 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48:K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="4">
         <v>0</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="4">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="K4" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="5">
         <v>2</v>
       </c>
-      <c r="J5" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="K5" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="5">
         <v>3</v>
       </c>
-      <c r="J6" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="K6" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="5">
         <v>4</v>
       </c>
-      <c r="J7" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="K7" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="5">
         <v>5</v>
       </c>
-      <c r="J8" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="K8" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="5">
         <v>6</v>
       </c>
-      <c r="J9" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="K9" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="5">
         <v>7</v>
       </c>
-      <c r="J10" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="K10" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="5">
         <v>8</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="5">
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="5">
         <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="5">
         <v>9</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="5">
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="5">
         <v>10</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="5">
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="F14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="5">
         <v>11</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="5">
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="5">
         <v>11</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="G15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="5">
         <v>12</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="5">
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="5">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="H16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="5">
         <v>13</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="5">
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="5">
         <v>13</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="1">
+      <c r="I17" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="5">
         <v>14</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="5">
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="5">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="1">
+      <c r="J18" s="4"/>
+      <c r="K18" s="5">
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J19" s="1">
+      <c r="B19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="5">
         <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0</v>
+      </c>
+      <c r="K30" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="4">
+        <v>1</v>
+      </c>
+      <c r="K32" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="5">
+        <v>2</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" s="5">
+        <v>2</v>
+      </c>
+      <c r="K33" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="5">
+        <v>3</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="5">
+        <v>3</v>
+      </c>
+      <c r="K34" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="5">
+        <v>4</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" s="5">
+        <v>4</v>
+      </c>
+      <c r="K35" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="5">
+        <v>5</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J36" s="5">
+        <v>5</v>
+      </c>
+      <c r="K36" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="5">
+        <v>6</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37" s="5">
+        <v>6</v>
+      </c>
+      <c r="K37" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="5">
+        <v>7</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J38" s="5">
+        <v>7</v>
+      </c>
+      <c r="K38" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J39" s="5">
+        <v>8</v>
+      </c>
+      <c r="K39" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="5">
+        <v>8</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J40" s="5">
+        <v>9</v>
+      </c>
+      <c r="K40" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="5">
+        <v>9</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J41" s="5">
+        <v>10</v>
+      </c>
+      <c r="K41" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="5">
+        <v>10</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J42" s="5">
+        <v>11</v>
+      </c>
+      <c r="K42" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="5">
+        <v>11</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J43" s="5">
+        <v>12</v>
+      </c>
+      <c r="K43" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="5">
+        <v>12</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J44" s="5">
+        <v>13</v>
+      </c>
+      <c r="K44" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="5">
+        <v>13</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J45" s="5">
+        <v>14</v>
+      </c>
+      <c r="K45" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="5">
+        <v>14</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J46" s="4"/>
+      <c r="K46" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K47" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>